<commit_message>
Method of Hierarchy Analysis
</commit_message>
<xml_diff>
--- a/out/Глобальные приоритеты.xlsx
+++ b/out/Глобальные приоритеты.xlsx
@@ -434,85 +434,100 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20.4" customWidth="1" min="1" max="1"/>
-    <col width="26.4" customWidth="1" min="2" max="2"/>
-    <col width="42" customWidth="1" min="3" max="3"/>
-    <col width="24" customWidth="1" min="4" max="4"/>
-    <col width="26.4" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="20.4" customWidth="1" min="7" max="7"/>
-    <col width="21.6" customWidth="1" min="8" max="8"/>
-    <col width="25.2" customWidth="1" min="9" max="9"/>
-    <col width="36" customWidth="1" min="10" max="10"/>
+    <col width="14.4" customWidth="1" min="1" max="1"/>
+    <col width="13.2" customWidth="1" min="2" max="2"/>
+    <col width="16.8" customWidth="1" min="3" max="3"/>
+    <col width="14.4" customWidth="1" min="4" max="4"/>
+    <col width="16.8" customWidth="1" min="5" max="5"/>
+    <col width="10.8" customWidth="1" min="6" max="6"/>
+    <col width="10.8" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="10.8" customWidth="1" min="9" max="9"/>
+    <col width="14.4" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Стоимость ТС (0.327)</t>
+          <t>Стоимость
+ТС
+(0.328)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Стоимость обслуживания ТС (0.157)</t>
+          <t>Стоимость
+обслуживания
+ТС
+(0.159)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Надёжность (0.227)</t>
+          <t>Надёжность
+(0.232)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Безопасность (0.108)</t>
+          <t>Безопасность
+(0.107)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Дизайн (0.05)</t>
+          <t>Дизайн
+(0.048)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Комфорт (0.073)</t>
+          <t>Комфорт
+(0.071)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Мощность (0.034)</t>
+          <t>Мощность
+(0.033)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Год выпуска (0.024)</t>
+          <t>Год
+выпуска
+(0.023)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Глобальные приоритеты выбора</t>
+          <t>Глобальные
+приоритеты
+выбора</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Kia Rio</t>
+          <t>Kia
+Rio</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>0.275</t>
+          <t>0.276</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>0.178</t>
+          <t>0.179</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>0.098</t>
+          <t>0.097</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -537,29 +552,30 @@
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>0.221</t>
+          <t>0.222</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>0.170</t>
+          <t>0.166</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Volkswagen Golf</t>
+          <t>Volkswagen
+Golf</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>0.094</t>
+          <t>0.092</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>0.102</t>
+          <t>0.101</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
@@ -574,7 +590,7 @@
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>0.227</t>
+          <t>0.228</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -584,44 +600,45 @@
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>0.227</t>
+          <t>0.228</t>
         </is>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>0.093</t>
+          <t>0.092</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
-          <t>0.110</t>
+          <t>0.104</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Toyota Corolla</t>
+          <t>Toyota
+Corolla</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>0.156</t>
+          <t>0.157</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>0.317</t>
+          <t>0.316</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>0.247</t>
+          <t>0.249</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>0.227</t>
+          <t>0.228</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
@@ -631,7 +648,7 @@
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>0.227</t>
+          <t>0.228</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
@@ -646,29 +663,30 @@
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>0.220</t>
+          <t>0.218</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Skoda Octavia</t>
+          <t>Skoda
+Octavia</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>0.156</t>
+          <t>0.157</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>0.178</t>
+          <t>0.179</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>0.158</t>
+          <t>0.157</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
@@ -693,29 +711,31 @@
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>0.221</t>
+          <t>0.222</t>
         </is>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>0.160</t>
+          <t>0.155</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>BMW 3 Series</t>
+          <t>BMW
+3
+Series</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>0.044</t>
+          <t>0.043</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>0.046</t>
+          <t>0.045</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
@@ -725,22 +745,22 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>0.361</t>
+          <t>0.362</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>0.361</t>
+          <t>0.362</t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>0.361</t>
+          <t>0.362</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
         <is>
-          <t>0.361</t>
+          <t>0.362</t>
         </is>
       </c>
       <c r="I6" s="1" t="inlineStr">
@@ -750,24 +770,25 @@
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>0.200</t>
+          <t>0.204</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Hyundai Solaris</t>
+          <t>Hyundai
+Solaris</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>0.275</t>
+          <t>0.276</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>0.178</t>
+          <t>0.179</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
@@ -797,12 +818,12 @@
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>0.093</t>
+          <t>0.092</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>0.150</t>
+          <t>0.154</t>
         </is>
       </c>
     </row>

</xml_diff>